<commit_message>
Updated code with diagnostics feature
</commit_message>
<xml_diff>
--- a/doc/text_to_voice_requirements.xlsx
+++ b/doc/text_to_voice_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91843\RWTV\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\108449\Downloads\personal\dev\RWTV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{424A1746-33CE-466E-9E10-372FEE9E4CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C2E185-BE73-45F0-AFFD-3D2AD7E1DED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="828" windowWidth="23040" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>System</t>
   </si>
@@ -43,116 +43,74 @@
     <t>Speech Processing</t>
   </si>
   <si>
-    <t>Text-to-Speech</t>
-  </si>
-  <si>
-    <t>RWS00001</t>
-  </si>
-  <si>
-    <t>RWS00002</t>
-  </si>
-  <si>
-    <t>RWS00003</t>
-  </si>
-  <si>
-    <t>RWS00004</t>
-  </si>
-  <si>
-    <t>RWS00005</t>
-  </si>
-  <si>
-    <t>RWS00006</t>
-  </si>
-  <si>
-    <t>RWS00007</t>
-  </si>
-  <si>
-    <t>RWS00008</t>
-  </si>
-  <si>
-    <t>RWS00009</t>
-  </si>
-  <si>
-    <t>RWS00010</t>
-  </si>
-  <si>
-    <t>RWS00011</t>
-  </si>
-  <si>
-    <t>RWS00012</t>
-  </si>
-  <si>
-    <t>RWS00013</t>
-  </si>
-  <si>
-    <t>RWS00014</t>
-  </si>
-  <si>
-    <t>RWS00015</t>
-  </si>
-  <si>
-    <t>RWS00016</t>
-  </si>
-  <si>
-    <t>RWS00017</t>
-  </si>
-  <si>
-    <t>The system should check function name.</t>
-  </si>
-  <si>
-    <t>The system should verify input text handling.</t>
-  </si>
-  <si>
-    <t>The system should test empty input handling.</t>
-  </si>
-  <si>
-    <t>The system should test long text input.</t>
-  </si>
-  <si>
-    <t>The system should test special character handling.</t>
-  </si>
-  <si>
-    <t>The system should check mp3 format support.</t>
-  </si>
-  <si>
-    <t>The system should check wav format support.</t>
-  </si>
-  <si>
-    <t>The system should verify base64 encoding.</t>
-  </si>
-  <si>
-    <t>The system should verify base64 decoding.</t>
-  </si>
-  <si>
-    <t>The system should verify speech playback.</t>
-  </si>
-  <si>
-    <t>The system should test response format.</t>
-  </si>
-  <si>
-    <t>The system should test language support.</t>
-  </si>
-  <si>
-    <t>The system should check for invalid text inputs.</t>
-  </si>
-  <si>
-    <t>The system should check punctuation handling.</t>
-  </si>
-  <si>
-    <t>The system should check performance for long text.</t>
-  </si>
-  <si>
-    <t>The system should verify system logs.</t>
-  </si>
-  <si>
-    <t>The system should check exception handling.</t>
+    <t>The function name should be text_to_speech()</t>
+  </si>
+  <si>
+    <t>The function should accept a text input parameter</t>
+  </si>
+  <si>
+    <t>The function should convert the text into speech using a selected TTS engin</t>
+  </si>
+  <si>
+    <t>The output audio file format should be MP3, wav</t>
+  </si>
+  <si>
+    <t>The function should return the audio after successful conversion</t>
+  </si>
+  <si>
+    <t>The function should handle errors such as empty input or unsupported characters</t>
+  </si>
+  <si>
+    <t>The function should support multiple languages if configured</t>
+  </si>
+  <si>
+    <t>The function should allow adjusting speech parameters like pitch and speed</t>
+  </si>
+  <si>
+    <t>The server should respond with SUCCESS if the speech is generated successfully</t>
+  </si>
+  <si>
+    <t>The server should respond with an error if invalid input is provided</t>
+  </si>
+  <si>
+    <t>RWTV00001</t>
+  </si>
+  <si>
+    <t>RWTV00002</t>
+  </si>
+  <si>
+    <t>RWTV00003</t>
+  </si>
+  <si>
+    <t>RWTV00004</t>
+  </si>
+  <si>
+    <t>RWTV00005</t>
+  </si>
+  <si>
+    <t>RWTV00006</t>
+  </si>
+  <si>
+    <t>RWTV00007</t>
+  </si>
+  <si>
+    <t>RWTV00008</t>
+  </si>
+  <si>
+    <t>RWTV00009</t>
+  </si>
+  <si>
+    <t>RWTV00010</t>
+  </si>
+  <si>
+    <t>Text-to-Voice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +122,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -224,6 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,7 +496,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,7 +504,7 @@
     <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
     <col min="5" max="5" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -568,190 +533,148 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
+      <c r="D10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -759,6 +682,7 @@
     <mergeCell ref="B2:B18"/>
     <mergeCell ref="C2:C18"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>